<commit_message>
add different code for each attempt from chatgpt, add settings for python default formatter
</commit_message>
<xml_diff>
--- a/pertemuan-11 (certainty factor dengan excel)/latihan/jumat (dari pak sendi).xlsx
+++ b/pertemuan-11 (certainty factor dengan excel)/latihan/jumat (dari pak sendi).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\Kuliah\Genap\KECERDASAN BUATAN 2023\SLIDES\TM 10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIGABYTE-B550\Documents\kecerdasan-buatan-program\pertemuan-11 (certainty factor dengan excel)\latihan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B44DACF-6E4F-4665-9617-C4567DA6B40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93628133-201D-4A70-BE0C-4A50834D029A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30936" yWindow="168" windowWidth="13212" windowHeight="12336" activeTab="4" xr2:uid="{5CC9C8C1-DCB5-4D49-8798-9AC44A0E459D}"/>
+    <workbookView xWindow="2820" yWindow="2970" windowWidth="21600" windowHeight="11835" xr2:uid="{5CC9C8C1-DCB5-4D49-8798-9AC44A0E459D}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -333,12 +333,6 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -352,6 +346,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA2B0CF-5C4D-4179-B9A2-2A3A85FE50B5}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,200 +685,200 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="F4" s="2" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="F4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <v>1</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="2">
         <v>0.8</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="2">
         <v>2</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="2">
         <v>2</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="2">
         <v>0.6</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="2">
         <v>3</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="2">
         <v>3</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="2" t="s">
         <v>23</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="2">
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="2">
         <v>4</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="2">
         <v>4</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="2">
         <v>0.2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F10" s="4">
+      <c r="F10" s="2">
         <v>5</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="2">
         <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F11" s="4">
+      <c r="F11" s="2">
         <v>6</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="2" t="s">
         <v>29</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="2">
         <v>0.5</v>
       </c>
     </row>
@@ -899,7 +899,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C7"/>
+      <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,18 +970,18 @@
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="str" cm="1">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="str" cm="1">
         <f t="array" ref="A1:B1">Pasien!A3:B3</f>
         <v>Pusing</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1" s="4">
         <v>0.5</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1013,18 +1013,18 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="str" cm="1">
+    <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="str" cm="1">
         <f t="array" ref="A5:B5">Pasien!A4:B4</f>
         <v>Batuk</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <v>0.8</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1056,18 +1056,18 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="str" cm="1">
+    <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="str" cm="1">
         <f t="array" ref="A9:B9">Pasien!A5:B5</f>
         <v>Dehidrasi</v>
       </c>
-      <c r="B9" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1099,21 +1099,21 @@
         <v>8.0000000000000016E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="str" cm="1">
+    <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="str" cm="1">
         <f t="array" ref="A13:B13">Pasien!A6:B6</f>
         <v>Keringan Dingin</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="4">
         <v>0.3</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="7"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1143,18 +1143,18 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="str" cm="1">
+    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="str" cm="1">
         <f t="array" ref="A17:B17">Pasien!A7:B7</f>
         <v>Menggigil</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="4">
         <v>0.2</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56848CE6-F80B-4D95-B750-4C15116E0FDB}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
@@ -1522,324 +1522,324 @@
       <c r="B22">
         <v>4</v>
       </c>
-      <c r="C22" s="10">
-        <v>0.4</v>
-      </c>
-      <c r="D22" s="10">
-        <v>0.4</v>
-      </c>
-      <c r="E22" s="10">
+      <c r="C22" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="E22" s="8">
         <v>0.08</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="8">
         <v>0.18</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="4">
         <f>C22</f>
         <v>0.4</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="4">
         <f>D22</f>
         <v>0.4</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="4">
         <f>B24</f>
         <v>0.4</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H24" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4">
         <f>B24</f>
         <v>0.4</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="4">
         <f>D24</f>
         <v>0.4</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="4">
         <f>1-B25</f>
         <v>0.6</v>
       </c>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4">
         <f>B25</f>
         <v>0.4</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="4">
         <f>D25*F25</f>
         <v>0.24</v>
       </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4">
         <f>B26+D26</f>
         <v>0.64</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="4">
         <f>B27*100</f>
         <v>64</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <f>B27</f>
         <v>0.64</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <f>E22</f>
         <v>0.08</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="6">
         <f>B30</f>
         <v>0.64</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H30" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6">
         <f>B30</f>
         <v>0.64</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="6">
         <f>D30</f>
         <v>0.08</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="6">
         <f>1-B31</f>
         <v>0.36</v>
       </c>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6">
         <f>B31</f>
         <v>0.64</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="6">
         <f>D31*F31</f>
         <v>2.8799999999999999E-2</v>
       </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6">
         <f>B32+D32</f>
         <v>0.66880000000000006</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="6">
         <f>B33*100</f>
         <v>66.88000000000001</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B36" s="7">
         <f>B33</f>
         <v>0.66880000000000006</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="7">
         <f>F22</f>
         <v>0.18</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E36" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="F36" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="7">
         <f>B36</f>
         <v>0.66880000000000006</v>
       </c>
-      <c r="H36" s="9" t="s">
+      <c r="H36" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="9">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7">
         <f>B36</f>
         <v>0.66880000000000006</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="7">
         <f>D36</f>
         <v>0.18</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E37" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F37" s="9">
+      <c r="F37" s="7">
         <f>1-B37</f>
         <v>0.33119999999999994</v>
       </c>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="9">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7">
         <f>B37</f>
         <v>0.66880000000000006</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D38" s="7">
         <f>D37*F37</f>
         <v>5.9615999999999988E-2</v>
       </c>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7">
         <f>B38+D38</f>
         <v>0.72841600000000006</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39" s="7">
         <f>B39*100</f>
         <v>72.8416</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E39" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="str" cm="1">
@@ -1890,8 +1890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AFCDAB6-5121-4970-B503-76E48F45AA75}">
   <dimension ref="A2:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1931,18 +1931,18 @@
         <v>26.200000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="6" cm="1">
+      <c r="B6" s="4" cm="1">
         <f t="array" ref="B6:C6">'Proses Lanjut'!D39:E39</f>
         <v>72.8416</v>
       </c>
-      <c r="C6" s="6" t="str">
+      <c r="C6" s="4" t="str">
         <v>%</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <v>72.8416</v>
       </c>
     </row>

</xml_diff>